<commit_message>
Update trending hashtags - 2026-02-21 [html]
</commit_message>
<xml_diff>
--- a/tiktok_hashtags_20260221.xlsx
+++ b/tiktok_hashtags_20260221.xlsx
@@ -492,7 +492,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -592,7 +592,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -617,7 +617,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -642,7 +642,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -692,7 +692,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -717,7 +717,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -742,7 +742,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -767,7 +767,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -792,7 +792,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -817,7 +817,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -867,7 +867,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -892,7 +892,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -917,7 +917,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -942,7 +942,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -967,7 +967,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -992,7 +992,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1092,7 +1092,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1217,7 +1217,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1242,7 +1242,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1292,7 +1292,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1442,7 +1442,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1542,7 +1542,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1567,7 +1567,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1592,7 +1592,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1617,7 +1617,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1642,7 +1642,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1717,7 +1717,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1742,7 +1742,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1767,7 +1767,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1817,7 +1817,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -1992,7 +1992,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2017,7 +2017,7 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2067,7 +2067,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2092,7 +2092,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2117,7 +2117,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2192,7 +2192,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2242,7 +2242,7 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2292,7 +2292,7 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2317,7 +2317,7 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2392,7 +2392,7 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2417,7 +2417,7 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2442,7 +2442,7 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2492,7 +2492,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2517,7 +2517,7 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2567,7 +2567,7 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -2667,7 +2667,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -2717,7 +2717,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -2742,7 +2742,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -2842,7 +2842,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -2867,7 +2867,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -2892,7 +2892,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -2917,7 +2917,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -2942,7 +2942,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -2992,7 +2992,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -3138,7 +3138,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -3163,7 +3163,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -3188,7 +3188,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -3213,7 +3213,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -3238,7 +3238,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -3288,7 +3288,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -3438,7 +3438,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -3463,7 +3463,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -3513,7 +3513,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -3538,7 +3538,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -3588,7 +3588,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -3659,7 +3659,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3684,7 +3684,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -3759,7 +3759,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -3784,7 +3784,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -3834,7 +3834,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -3859,7 +3859,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -3884,7 +3884,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -3934,7 +3934,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -4005,7 +4005,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -4030,7 +4030,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -4055,7 +4055,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -4080,7 +4080,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -4105,7 +4105,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -4130,7 +4130,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -4155,7 +4155,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -4205,7 +4205,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4230,7 +4230,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -4255,7 +4255,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -4280,7 +4280,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -4351,7 +4351,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -4376,7 +4376,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -4451,7 +4451,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -4476,7 +4476,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -4501,7 +4501,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -4526,7 +4526,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -4551,7 +4551,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4576,7 +4576,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -4601,7 +4601,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -4672,7 +4672,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -4722,7 +4722,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -4747,7 +4747,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -4772,7 +4772,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -4797,7 +4797,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -4822,7 +4822,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -4847,7 +4847,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -4872,7 +4872,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -4922,7 +4922,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -4993,7 +4993,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -5018,7 +5018,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -5043,7 +5043,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -5068,7 +5068,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -5143,7 +5143,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -5168,7 +5168,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -5193,7 +5193,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -5218,7 +5218,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -5243,7 +5243,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -5268,7 +5268,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -5364,7 +5364,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -5389,7 +5389,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -5414,7 +5414,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -5439,7 +5439,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -5464,7 +5464,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -5489,7 +5489,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -5514,7 +5514,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -5539,7 +5539,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -5564,7 +5564,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -5589,7 +5589,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -5660,7 +5660,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -5685,7 +5685,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -5710,7 +5710,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -5735,7 +5735,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -5760,7 +5760,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -5785,7 +5785,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -5810,7 +5810,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -5835,7 +5835,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -5860,7 +5860,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -5885,7 +5885,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -5910,7 +5910,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -5935,7 +5935,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2026-02-21 21:19:38</t>
+          <t>2026-02-21 21:23:34</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">

</xml_diff>